<commit_message>
inclusão das datas de reaberturas nos graficos diarios
</commit_message>
<xml_diff>
--- a/docs/excel_sp.xlsx
+++ b/docs/excel_sp.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="120">
   <si>
     <t>02/25/20</t>
   </si>
@@ -315,6 +315,12 @@
     <t>06/03/20</t>
   </si>
   <si>
+    <t>06/04/20</t>
+  </si>
+  <si>
+    <t>06/05/20</t>
+  </si>
+  <si>
     <t>CASO SEM LOCALIZAÇÃO DEFINIDA/SP</t>
   </si>
   <si>
@@ -719,10 +725,16 @@
       <c r="CW1" t="s">
         <v>99</v>
       </c>
+      <c r="CX1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B2" t="n">
         <v>0.0</v>
@@ -1023,11 +1035,17 @@
       </c>
       <c r="CW2" t="n">
         <v>79.0</v>
+      </c>
+      <c r="CX2" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="CY2" t="n">
+        <v>5445.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B3" t="n">
         <v>0.0</v>
@@ -1328,11 +1346,17 @@
       </c>
       <c r="CW3" t="n">
         <v>485.0</v>
+      </c>
+      <c r="CX3" t="n">
+        <v>505.0</v>
+      </c>
+      <c r="CY3" t="n">
+        <v>505.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B4" t="n">
         <v>0.0</v>
@@ -1633,11 +1657,17 @@
       </c>
       <c r="CW4" t="n">
         <v>459.0</v>
+      </c>
+      <c r="CX4" t="n">
+        <v>478.0</v>
+      </c>
+      <c r="CY4" t="n">
+        <v>478.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B5" t="n">
         <v>0.0</v>
@@ -1938,11 +1968,17 @@
       </c>
       <c r="CW5" t="n">
         <v>1167.0</v>
+      </c>
+      <c r="CX5" t="n">
+        <v>1257.0</v>
+      </c>
+      <c r="CY5" t="n">
+        <v>1257.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B6" t="n">
         <v>0.0</v>
@@ -2243,11 +2279,17 @@
       </c>
       <c r="CW6" t="n">
         <v>7889.0</v>
+      </c>
+      <c r="CX6" t="n">
+        <v>8408.0</v>
+      </c>
+      <c r="CY6" t="n">
+        <v>8408.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B7" t="n">
         <v>0.0</v>
@@ -2548,11 +2590,17 @@
       </c>
       <c r="CW7" t="n">
         <v>741.0</v>
+      </c>
+      <c r="CX7" t="n">
+        <v>793.0</v>
+      </c>
+      <c r="CY7" t="n">
+        <v>793.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B8" t="n">
         <v>0.0</v>
@@ -2853,11 +2901,17 @@
       </c>
       <c r="CW8" t="n">
         <v>248.0</v>
+      </c>
+      <c r="CX8" t="n">
+        <v>265.0</v>
+      </c>
+      <c r="CY8" t="n">
+        <v>265.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B9" t="n">
         <v>0.0</v>
@@ -3158,11 +3212,17 @@
       </c>
       <c r="CW9" t="n">
         <v>245.0</v>
+      </c>
+      <c r="CX9" t="n">
+        <v>255.0</v>
+      </c>
+      <c r="CY9" t="n">
+        <v>255.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B10" t="n">
         <v>0.0</v>
@@ -3463,11 +3523,17 @@
       </c>
       <c r="CW10" t="n">
         <v>396.0</v>
+      </c>
+      <c r="CX10" t="n">
+        <v>430.0</v>
+      </c>
+      <c r="CY10" t="n">
+        <v>430.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B11" t="n">
         <v>0.0</v>
@@ -3768,11 +3834,17 @@
       </c>
       <c r="CW11" t="n">
         <v>561.0</v>
+      </c>
+      <c r="CX11" t="n">
+        <v>586.0</v>
+      </c>
+      <c r="CY11" t="n">
+        <v>586.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B12" t="n">
         <v>0.0</v>
@@ -4073,11 +4145,17 @@
       </c>
       <c r="CW12" t="n">
         <v>531.0</v>
+      </c>
+      <c r="CX12" t="n">
+        <v>559.0</v>
+      </c>
+      <c r="CY12" t="n">
+        <v>559.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B13" t="n">
         <v>0.0</v>
@@ -4378,11 +4456,17 @@
       </c>
       <c r="CW13" t="n">
         <v>1458.0</v>
+      </c>
+      <c r="CX13" t="n">
+        <v>1515.0</v>
+      </c>
+      <c r="CY13" t="n">
+        <v>1515.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B14" t="n">
         <v>0.0</v>
@@ -4683,11 +4767,17 @@
       </c>
       <c r="CW14" t="n">
         <v>8063.0</v>
+      </c>
+      <c r="CX14" t="n">
+        <v>8615.0</v>
+      </c>
+      <c r="CY14" t="n">
+        <v>8615.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B15" t="n">
         <v>0.0</v>
@@ -4988,11 +5078,17 @@
       </c>
       <c r="CW15" t="n">
         <v>1557.0</v>
+      </c>
+      <c r="CX15" t="n">
+        <v>1680.0</v>
+      </c>
+      <c r="CY15" t="n">
+        <v>1680.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B16" t="n">
         <v>0.0</v>
@@ -5293,11 +5389,17 @@
       </c>
       <c r="CW16" t="n">
         <v>2392.0</v>
+      </c>
+      <c r="CX16" t="n">
+        <v>2528.0</v>
+      </c>
+      <c r="CY16" t="n">
+        <v>2528.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B17" t="n">
         <v>0.0</v>
@@ -5598,11 +5700,17 @@
       </c>
       <c r="CW17" t="n">
         <v>3020.0</v>
+      </c>
+      <c r="CX17" t="n">
+        <v>3188.0</v>
+      </c>
+      <c r="CY17" t="n">
+        <v>3188.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B18" t="n">
         <v>1.0</v>
@@ -5903,11 +6011,17 @@
       </c>
       <c r="CW18" t="n">
         <v>94192.0</v>
+      </c>
+      <c r="CX18" t="n">
+        <v>98058.0</v>
+      </c>
+      <c r="CY18" t="n">
+        <v>98058.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B19" t="n">
         <v>1.0</v>
@@ -6208,6 +6322,12 @@
       </c>
       <c r="CW19" t="n">
         <v>66777.0</v>
+      </c>
+      <c r="CX19" t="n">
+        <v>69347.0</v>
+      </c>
+      <c r="CY19" t="n">
+        <v>69347.0</v>
       </c>
     </row>
   </sheetData>
@@ -6525,10 +6645,16 @@
       <c r="CW1" t="s">
         <v>99</v>
       </c>
+      <c r="CX1" t="s">
+        <v>100</v>
+      </c>
+      <c r="CY1" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B2" t="n">
         <v>0.0</v>
@@ -6829,11 +6955,17 @@
       </c>
       <c r="CW2" t="n">
         <v>0.0</v>
+      </c>
+      <c r="CX2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="CY2" t="n">
+        <v>281.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B3" t="n">
         <v>0.0</v>
@@ -7134,11 +7266,17 @@
       </c>
       <c r="CW3" t="n">
         <v>26.0</v>
+      </c>
+      <c r="CX3" t="n">
+        <v>28.0</v>
+      </c>
+      <c r="CY3" t="n">
+        <v>28.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B4" t="n">
         <v>0.0</v>
@@ -7439,11 +7577,17 @@
       </c>
       <c r="CW4" t="n">
         <v>22.0</v>
+      </c>
+      <c r="CX4" t="n">
+        <v>24.0</v>
+      </c>
+      <c r="CY4" t="n">
+        <v>24.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B5" t="n">
         <v>0.0</v>
@@ -7744,11 +7888,17 @@
       </c>
       <c r="CW5" t="n">
         <v>50.0</v>
+      </c>
+      <c r="CX5" t="n">
+        <v>52.0</v>
+      </c>
+      <c r="CY5" t="n">
+        <v>52.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B6" t="n">
         <v>0.0</v>
@@ -8049,11 +8199,17 @@
       </c>
       <c r="CW6" t="n">
         <v>388.0</v>
+      </c>
+      <c r="CX6" t="n">
+        <v>414.0</v>
+      </c>
+      <c r="CY6" t="n">
+        <v>414.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B7" t="n">
         <v>0.0</v>
@@ -8353,12 +8509,18 @@
         <v>17.0</v>
       </c>
       <c r="CW7" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="CX7" t="n">
+        <v>17.0</v>
+      </c>
+      <c r="CY7" t="n">
         <v>17.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B8" t="n">
         <v>0.0</v>
@@ -8659,11 +8821,17 @@
       </c>
       <c r="CW8" t="n">
         <v>8.0</v>
+      </c>
+      <c r="CX8" t="n">
+        <v>9.0</v>
+      </c>
+      <c r="CY8" t="n">
+        <v>9.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B9" t="n">
         <v>0.0</v>
@@ -8963,12 +9131,18 @@
         <v>15.0</v>
       </c>
       <c r="CW9" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="CX9" t="n">
+        <v>16.0</v>
+      </c>
+      <c r="CY9" t="n">
         <v>16.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B10" t="n">
         <v>0.0</v>
@@ -9269,11 +9443,17 @@
       </c>
       <c r="CW10" t="n">
         <v>16.0</v>
+      </c>
+      <c r="CX10" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="CY10" t="n">
+        <v>18.0</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B11" t="n">
         <v>0.0</v>
@@ -9574,11 +9754,17 @@
       </c>
       <c r="CW11" t="n">
         <v>42.0</v>
+      </c>
+      <c r="CX11" t="n">
+        <v>43.0</v>
+      </c>
+      <c r="CY11" t="n">
+        <v>43.0</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B12" t="n">
         <v>0.0</v>
@@ -9878,12 +10064,18 @@
         <v>18.0</v>
       </c>
       <c r="CW12" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="CX12" t="n">
+        <v>18.0</v>
+      </c>
+      <c r="CY12" t="n">
         <v>18.0</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B13" t="n">
         <v>0.0</v>
@@ -10184,11 +10376,17 @@
       </c>
       <c r="CW13" t="n">
         <v>56.0</v>
+      </c>
+      <c r="CX13" t="n">
+        <v>57.0</v>
+      </c>
+      <c r="CY13" t="n">
+        <v>57.0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B14" t="n">
         <v>0.0</v>
@@ -10489,11 +10687,17 @@
       </c>
       <c r="CW14" t="n">
         <v>435.0</v>
+      </c>
+      <c r="CX14" t="n">
+        <v>465.0</v>
+      </c>
+      <c r="CY14" t="n">
+        <v>465.0</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B15" t="n">
         <v>0.0</v>
@@ -10794,11 +10998,17 @@
       </c>
       <c r="CW15" t="n">
         <v>63.0</v>
+      </c>
+      <c r="CX15" t="n">
+        <v>66.0</v>
+      </c>
+      <c r="CY15" t="n">
+        <v>66.0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B16" t="n">
         <v>0.0</v>
@@ -11099,11 +11309,17 @@
       </c>
       <c r="CW16" t="n">
         <v>90.0</v>
+      </c>
+      <c r="CX16" t="n">
+        <v>97.0</v>
+      </c>
+      <c r="CY16" t="n">
+        <v>97.0</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B17" t="n">
         <v>0.0</v>
@@ -11404,11 +11620,17 @@
       </c>
       <c r="CW17" t="n">
         <v>148.0</v>
+      </c>
+      <c r="CX17" t="n">
+        <v>158.0</v>
+      </c>
+      <c r="CY17" t="n">
+        <v>158.0</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B18" t="n">
         <v>0.0</v>
@@ -11709,11 +11931,17 @@
       </c>
       <c r="CW18" t="n">
         <v>6881.0</v>
+      </c>
+      <c r="CX18" t="n">
+        <v>7079.0</v>
+      </c>
+      <c r="CY18" t="n">
+        <v>7079.0</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B19" t="n">
         <v>0.0</v>
@@ -12014,6 +12242,12 @@
       </c>
       <c r="CW19" t="n">
         <v>4564.0</v>
+      </c>
+      <c r="CX19" t="n">
+        <v>4675.0</v>
+      </c>
+      <c r="CY19" t="n">
+        <v>4675.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>